<commit_message>
Adición de naturaleza de cuentas
</commit_message>
<xml_diff>
--- a/Sistema Contable.xlsx
+++ b/Sistema Contable.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20736" windowHeight="11160" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20736" windowHeight="11160" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Configuraciones" sheetId="1" r:id="rId1"/>
@@ -13,9 +13,11 @@
     <sheet name="Balance general" sheetId="5" r:id="rId4"/>
     <sheet name="Estado de resultados" sheetId="6" r:id="rId5"/>
     <sheet name="Referencias" sheetId="3" r:id="rId6"/>
+    <sheet name="Tablas auxiliares" sheetId="7" r:id="rId7"/>
   </sheets>
   <definedNames>
     <definedName name="TblCatalogoCuentas_Etiqueta">TblCatalogoCuentas[Etiqueta]</definedName>
+    <definedName name="TblNaturalezaCuentas_Aux">TblNaturalezaCuentas[Naturaleza de cuentas]</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
   <extLst>
@@ -32,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="170">
   <si>
     <t>Nivel maximo de cuentas</t>
   </si>
@@ -524,6 +526,24 @@
   </si>
   <si>
     <t>DÓLARES DE LOS ESTADOS UNIDOS DE AMÉRICA</t>
+  </si>
+  <si>
+    <t>Naturaleza</t>
+  </si>
+  <si>
+    <t>Naturaleza de cuentas</t>
+  </si>
+  <si>
+    <t>Deudora</t>
+  </si>
+  <si>
+    <t>Acreedora</t>
+  </si>
+  <si>
+    <t>Disminuyen su valor con anotaciones en el debe (se aumenta la deuda u obligación que la empresa tiene contraída) y aumenta su valor con anotaciones en el haber (disminuye la deuda u obligación contraída).</t>
+  </si>
+  <si>
+    <t>Aumentan su valor mediante anotaciones en el debe y disminuyen su valor mediante anotaciones en el haber.</t>
   </si>
 </sst>
 </file>
@@ -646,7 +666,18 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="11">
+  <dxfs count="12">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFFFFDD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
       <fill>
@@ -712,9 +743,6 @@
       </fill>
     </dxf>
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -760,23 +788,24 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="TblCatalogoCuentas" displayName="TblCatalogoCuentas" ref="A1:E146" totalsRowShown="0">
-  <autoFilter ref="A1:E146"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="TblCatalogoCuentas" displayName="TblCatalogoCuentas" ref="A1:F146" totalsRowShown="0">
+  <autoFilter ref="A1:F146"/>
   <sortState ref="A2:D38">
     <sortCondition ref="A1:A38"/>
   </sortState>
-  <tableColumns count="5">
-    <tableColumn id="1" name="Código" dataDxfId="9"/>
-    <tableColumn id="2" name="Código extendido" dataDxfId="10">
+  <tableColumns count="6">
+    <tableColumn id="1" name="Código" dataDxfId="10"/>
+    <tableColumn id="2" name="Código extendido" dataDxfId="11">
       <calculatedColumnFormula>TblCatalogoCuentas[[#This Row],[Código]] &amp; REPT(" ",Configuraciones!$B$4 - LEN(TblCatalogoCuentas[[#This Row],[Código]]))</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="3" name="Nivel">
       <calculatedColumnFormula>LEN(TblCatalogoCuentas[[#This Row],[Código]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="Descripción" dataDxfId="7"/>
-    <tableColumn id="5" name="Etiqueta" dataDxfId="8">
+    <tableColumn id="4" name="Descripción" dataDxfId="9"/>
+    <tableColumn id="5" name="Etiqueta" dataDxfId="1">
       <calculatedColumnFormula>TblCatalogoCuentas[[#This Row],[Código]] &amp; " - " &amp; TblCatalogoCuentas[[#This Row],[Descripción]]</calculatedColumnFormula>
     </tableColumn>
+    <tableColumn id="6" name="Naturaleza" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -786,15 +815,26 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="TblLibroDiario" displayName="TblLibroDiario" ref="A7:G9" totalsRowShown="0">
   <autoFilter ref="A7:G9"/>
   <tableColumns count="7">
-    <tableColumn id="1" name="Correlativo" dataDxfId="6">
+    <tableColumn id="1" name="Correlativo" dataDxfId="8">
       <calculatedColumnFormula>ROW(TblLibroDiario[[#This Row],[Correlativo]])-ROW(TblLibroDiario[[#Headers],[Correlativo]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" name="Fecha" dataDxfId="5"/>
-    <tableColumn id="3" name="Cuenta" dataDxfId="4"/>
-    <tableColumn id="4" name="Descripción" dataDxfId="3"/>
-    <tableColumn id="5" name="Referencia" dataDxfId="2"/>
-    <tableColumn id="6" name="Debe" dataDxfId="1"/>
-    <tableColumn id="7" name="Haber" dataDxfId="0"/>
+    <tableColumn id="2" name="Fecha" dataDxfId="7"/>
+    <tableColumn id="3" name="Cuenta" dataDxfId="6"/>
+    <tableColumn id="4" name="Descripción" dataDxfId="5"/>
+    <tableColumn id="5" name="Referencia" dataDxfId="4"/>
+    <tableColumn id="6" name="Debe" dataDxfId="3"/>
+    <tableColumn id="7" name="Haber" dataDxfId="2"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="TblNaturalezaCuentas" displayName="TblNaturalezaCuentas" ref="A1:B3" totalsRowShown="0">
+  <autoFilter ref="A1:B3"/>
+  <tableColumns count="2">
+    <tableColumn id="1" name="Naturaleza de cuentas"/>
+    <tableColumn id="2" name="Descripción"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1129,8 +1169,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I146"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1156,6 +1196,9 @@
       <c r="E1" t="s">
         <v>149</v>
       </c>
+      <c r="F1" t="s">
+        <v>164</v>
+      </c>
     </row>
     <row r="2" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="10">
@@ -1176,6 +1219,9 @@
         <f>TblCatalogoCuentas[[#This Row],[Código]] &amp; " - " &amp; TblCatalogoCuentas[[#This Row],[Descripción]]</f>
         <v xml:space="preserve">1 - ACTIVO </v>
       </c>
+      <c r="F2" s="7" t="s">
+        <v>166</v>
+      </c>
       <c r="I2" s="2"/>
     </row>
     <row r="3" spans="1:9" ht="15" x14ac:dyDescent="0.25">
@@ -1197,6 +1243,9 @@
         <f>TblCatalogoCuentas[[#This Row],[Código]] &amp; " - " &amp; TblCatalogoCuentas[[#This Row],[Descripción]]</f>
         <v xml:space="preserve">11 - ACTIVO CORRIENTE </v>
       </c>
+      <c r="F3" s="7" t="s">
+        <v>166</v>
+      </c>
       <c r="I3" s="2"/>
     </row>
     <row r="4" spans="1:9" ht="15" x14ac:dyDescent="0.25">
@@ -1218,6 +1267,9 @@
         <f>TblCatalogoCuentas[[#This Row],[Código]] &amp; " - " &amp; TblCatalogoCuentas[[#This Row],[Descripción]]</f>
         <v>111 - EFECTIVO Y EQUIVALENTES</v>
       </c>
+      <c r="F4" s="7" t="s">
+        <v>166</v>
+      </c>
       <c r="I4" s="3"/>
     </row>
     <row r="5" spans="1:9" ht="15" x14ac:dyDescent="0.25">
@@ -1239,6 +1291,9 @@
         <f>TblCatalogoCuentas[[#This Row],[Código]] &amp; " - " &amp; TblCatalogoCuentas[[#This Row],[Descripción]]</f>
         <v>111001 - CAJA</v>
       </c>
+      <c r="F5" s="7" t="s">
+        <v>166</v>
+      </c>
       <c r="H5" s="3"/>
     </row>
     <row r="6" spans="1:9" ht="15" x14ac:dyDescent="0.25">
@@ -1260,6 +1315,9 @@
         <f>TblCatalogoCuentas[[#This Row],[Código]] &amp; " - " &amp; TblCatalogoCuentas[[#This Row],[Descripción]]</f>
         <v>111002 - BANCOS</v>
       </c>
+      <c r="F6" s="7" t="s">
+        <v>166</v>
+      </c>
       <c r="H6" s="3"/>
     </row>
     <row r="7" spans="1:9" ht="15" x14ac:dyDescent="0.25">
@@ -1281,6 +1339,9 @@
         <f>TblCatalogoCuentas[[#This Row],[Código]] &amp; " - " &amp; TblCatalogoCuentas[[#This Row],[Descripción]]</f>
         <v>112 - CUENTAS POR COBRAR</v>
       </c>
+      <c r="F7" s="7" t="s">
+        <v>166</v>
+      </c>
       <c r="I7" s="3"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
@@ -1302,6 +1363,9 @@
         <f>TblCatalogoCuentas[[#This Row],[Código]] &amp; " - " &amp; TblCatalogoCuentas[[#This Row],[Descripción]]</f>
         <v xml:space="preserve">112001 - PRÉSTAMOS Y ANTICIPOS A EMPLEADOS </v>
       </c>
+      <c r="F8" s="7" t="s">
+        <v>166</v>
+      </c>
       <c r="H8" s="3"/>
     </row>
     <row r="9" spans="1:9" ht="15" x14ac:dyDescent="0.25">
@@ -1323,6 +1387,9 @@
         <f>TblCatalogoCuentas[[#This Row],[Código]] &amp; " - " &amp; TblCatalogoCuentas[[#This Row],[Descripción]]</f>
         <v xml:space="preserve">112002 - DOCUMENTOS POR COBRAR </v>
       </c>
+      <c r="F9" s="7" t="s">
+        <v>166</v>
+      </c>
       <c r="H9" s="3"/>
     </row>
     <row r="10" spans="1:9" ht="15" x14ac:dyDescent="0.25">
@@ -1344,6 +1411,9 @@
         <f>TblCatalogoCuentas[[#This Row],[Código]] &amp; " - " &amp; TblCatalogoCuentas[[#This Row],[Descripción]]</f>
         <v xml:space="preserve">112003 - IVA POR RECLAMAR </v>
       </c>
+      <c r="F10" s="7" t="s">
+        <v>166</v>
+      </c>
       <c r="H10" s="3"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
@@ -1365,6 +1435,9 @@
         <f>TblCatalogoCuentas[[#This Row],[Código]] &amp; " - " &amp; TblCatalogoCuentas[[#This Row],[Descripción]]</f>
         <v xml:space="preserve">112004 - ESTIMACIÓN PARA CUENTAS INCOBRABLES </v>
       </c>
+      <c r="F11" s="7" t="s">
+        <v>166</v>
+      </c>
       <c r="H11" s="3"/>
     </row>
     <row r="12" spans="1:9" ht="15" x14ac:dyDescent="0.25">
@@ -1386,6 +1459,9 @@
         <f>TblCatalogoCuentas[[#This Row],[Código]] &amp; " - " &amp; TblCatalogoCuentas[[#This Row],[Descripción]]</f>
         <v xml:space="preserve">113 - INVENTARIOS </v>
       </c>
+      <c r="F12" s="7" t="s">
+        <v>166</v>
+      </c>
       <c r="I12" s="3"/>
     </row>
     <row r="13" spans="1:9" ht="15" x14ac:dyDescent="0.25">
@@ -1407,6 +1483,9 @@
         <f>TblCatalogoCuentas[[#This Row],[Código]] &amp; " - " &amp; TblCatalogoCuentas[[#This Row],[Descripción]]</f>
         <v xml:space="preserve">113001 - INVENTARIO MORTADELA </v>
       </c>
+      <c r="F13" s="7" t="s">
+        <v>166</v>
+      </c>
       <c r="H13" s="3"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
@@ -1428,6 +1507,9 @@
         <f>TblCatalogoCuentas[[#This Row],[Código]] &amp; " - " &amp; TblCatalogoCuentas[[#This Row],[Descripción]]</f>
         <v xml:space="preserve">113002 - INVENTARIO JAMÓN </v>
       </c>
+      <c r="F14" s="7" t="s">
+        <v>166</v>
+      </c>
       <c r="H14" s="3"/>
     </row>
     <row r="15" spans="1:9" ht="15" x14ac:dyDescent="0.25">
@@ -1449,6 +1531,9 @@
         <f>TblCatalogoCuentas[[#This Row],[Código]] &amp; " - " &amp; TblCatalogoCuentas[[#This Row],[Descripción]]</f>
         <v>113003 - INVENTARIO CHORIZOS</v>
       </c>
+      <c r="F15" s="7" t="s">
+        <v>166</v>
+      </c>
       <c r="H15" s="3"/>
     </row>
     <row r="16" spans="1:9" ht="15" x14ac:dyDescent="0.25">
@@ -1470,6 +1555,9 @@
         <f>TblCatalogoCuentas[[#This Row],[Código]] &amp; " - " &amp; TblCatalogoCuentas[[#This Row],[Descripción]]</f>
         <v xml:space="preserve">113004 - INVENTARIO SALAMI </v>
       </c>
+      <c r="F16" s="7" t="s">
+        <v>166</v>
+      </c>
       <c r="H16" s="3"/>
     </row>
     <row r="17" spans="1:9" ht="15" x14ac:dyDescent="0.25">
@@ -1491,6 +1579,9 @@
         <f>TblCatalogoCuentas[[#This Row],[Código]] &amp; " - " &amp; TblCatalogoCuentas[[#This Row],[Descripción]]</f>
         <v>113005 - INVENTARIO SALCHICHAS</v>
       </c>
+      <c r="F17" s="7" t="s">
+        <v>166</v>
+      </c>
       <c r="H17" s="3"/>
     </row>
     <row r="18" spans="1:9" ht="15" x14ac:dyDescent="0.25">
@@ -1512,6 +1603,9 @@
         <f>TblCatalogoCuentas[[#This Row],[Código]] &amp; " - " &amp; TblCatalogoCuentas[[#This Row],[Descripción]]</f>
         <v xml:space="preserve">113006 - INVENTARIO CARNE EN CANAL </v>
       </c>
+      <c r="F18" s="7" t="s">
+        <v>166</v>
+      </c>
       <c r="H18" s="3"/>
     </row>
     <row r="19" spans="1:9" ht="15" x14ac:dyDescent="0.25">
@@ -1533,6 +1627,9 @@
         <f>TblCatalogoCuentas[[#This Row],[Código]] &amp; " - " &amp; TblCatalogoCuentas[[#This Row],[Descripción]]</f>
         <v>113007 - INVENTARIO CARNE DESPOSTADA</v>
       </c>
+      <c r="F19" s="7" t="s">
+        <v>166</v>
+      </c>
       <c r="H19" s="3"/>
     </row>
     <row r="20" spans="1:9" ht="15" x14ac:dyDescent="0.25">
@@ -1554,6 +1651,9 @@
         <f>TblCatalogoCuentas[[#This Row],[Código]] &amp; " - " &amp; TblCatalogoCuentas[[#This Row],[Descripción]]</f>
         <v xml:space="preserve">114 - PAGOS ANTICIPADOS </v>
       </c>
+      <c r="F20" s="7" t="s">
+        <v>166</v>
+      </c>
       <c r="I20" s="3"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.3">
@@ -1575,6 +1675,9 @@
         <f>TblCatalogoCuentas[[#This Row],[Código]] &amp; " - " &amp; TblCatalogoCuentas[[#This Row],[Descripción]]</f>
         <v xml:space="preserve">114001 - PAPELERÍA Y ÚTILES </v>
       </c>
+      <c r="F21" s="7" t="s">
+        <v>166</v>
+      </c>
       <c r="H21" s="3"/>
     </row>
     <row r="22" spans="1:9" ht="15" x14ac:dyDescent="0.25">
@@ -1596,6 +1699,9 @@
         <f>TblCatalogoCuentas[[#This Row],[Código]] &amp; " - " &amp; TblCatalogoCuentas[[#This Row],[Descripción]]</f>
         <v>114002 - SEGUROS PAGADOS POR ANTICIPADO</v>
       </c>
+      <c r="F22" s="7" t="s">
+        <v>166</v>
+      </c>
       <c r="H22" s="3"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.3">
@@ -1617,6 +1723,9 @@
         <f>TblCatalogoCuentas[[#This Row],[Código]] &amp; " - " &amp; TblCatalogoCuentas[[#This Row],[Descripción]]</f>
         <v xml:space="preserve">115 - IVA CRÉDITO FISCAL </v>
       </c>
+      <c r="F23" s="7" t="s">
+        <v>166</v>
+      </c>
       <c r="I23" s="3"/>
     </row>
     <row r="24" spans="1:9" ht="15" x14ac:dyDescent="0.25">
@@ -1638,6 +1747,9 @@
         <f>TblCatalogoCuentas[[#This Row],[Código]] &amp; " - " &amp; TblCatalogoCuentas[[#This Row],[Descripción]]</f>
         <v xml:space="preserve">12 - ACTIVO NO CORRIENTE </v>
       </c>
+      <c r="F24" s="7" t="s">
+        <v>166</v>
+      </c>
       <c r="I24" s="2"/>
     </row>
     <row r="25" spans="1:9" ht="15" x14ac:dyDescent="0.25">
@@ -1659,6 +1771,9 @@
         <f>TblCatalogoCuentas[[#This Row],[Código]] &amp; " - " &amp; TblCatalogoCuentas[[#This Row],[Descripción]]</f>
         <v xml:space="preserve">121 - PROPIEDAD, PLANTA Y EQUIPO </v>
       </c>
+      <c r="F25" s="7" t="s">
+        <v>166</v>
+      </c>
       <c r="I25" s="3"/>
     </row>
     <row r="26" spans="1:9" ht="15" x14ac:dyDescent="0.25">
@@ -1680,6 +1795,9 @@
         <f>TblCatalogoCuentas[[#This Row],[Código]] &amp; " - " &amp; TblCatalogoCuentas[[#This Row],[Descripción]]</f>
         <v>121001 - BIENES INMUEBLES</v>
       </c>
+      <c r="F26" s="7" t="s">
+        <v>166</v>
+      </c>
       <c r="H26" s="3"/>
     </row>
     <row r="27" spans="1:9" ht="15" x14ac:dyDescent="0.25">
@@ -1701,6 +1819,9 @@
         <f>TblCatalogoCuentas[[#This Row],[Código]] &amp; " - " &amp; TblCatalogoCuentas[[#This Row],[Descripción]]</f>
         <v xml:space="preserve">121001001 - TERRENOS </v>
       </c>
+      <c r="F27" s="7" t="s">
+        <v>166</v>
+      </c>
       <c r="H27" s="3"/>
     </row>
     <row r="28" spans="1:9" ht="15" x14ac:dyDescent="0.25">
@@ -1722,6 +1843,9 @@
         <f>TblCatalogoCuentas[[#This Row],[Código]] &amp; " - " &amp; TblCatalogoCuentas[[#This Row],[Descripción]]</f>
         <v xml:space="preserve">121001002 - INSTALACIONES </v>
       </c>
+      <c r="F28" s="7" t="s">
+        <v>166</v>
+      </c>
       <c r="H28" s="3"/>
     </row>
     <row r="29" spans="1:9" ht="15" x14ac:dyDescent="0.25">
@@ -1743,6 +1867,9 @@
         <f>TblCatalogoCuentas[[#This Row],[Código]] &amp; " - " &amp; TblCatalogoCuentas[[#This Row],[Descripción]]</f>
         <v xml:space="preserve">121002 - BIENES MUEBLES </v>
       </c>
+      <c r="F29" s="7" t="s">
+        <v>166</v>
+      </c>
       <c r="H29" s="3"/>
     </row>
     <row r="30" spans="1:9" ht="15" x14ac:dyDescent="0.25">
@@ -1764,6 +1891,9 @@
         <f>TblCatalogoCuentas[[#This Row],[Código]] &amp; " - " &amp; TblCatalogoCuentas[[#This Row],[Descripción]]</f>
         <v>121002001 - MOBILIARIO Y EQUIPO DE OFICINA</v>
       </c>
+      <c r="F30" s="7" t="s">
+        <v>166</v>
+      </c>
       <c r="H30" s="3"/>
     </row>
     <row r="31" spans="1:9" ht="15" x14ac:dyDescent="0.25">
@@ -1785,6 +1915,9 @@
         <f>TblCatalogoCuentas[[#This Row],[Código]] &amp; " - " &amp; TblCatalogoCuentas[[#This Row],[Descripción]]</f>
         <v>121002002 - MOBILIARIO Y EQUIPO DE VENTA</v>
       </c>
+      <c r="F31" s="7" t="s">
+        <v>166</v>
+      </c>
       <c r="H31" s="3"/>
     </row>
     <row r="32" spans="1:9" ht="15" x14ac:dyDescent="0.25">
@@ -1806,6 +1939,9 @@
         <f>TblCatalogoCuentas[[#This Row],[Código]] &amp; " - " &amp; TblCatalogoCuentas[[#This Row],[Descripción]]</f>
         <v xml:space="preserve">121002003 - EQUIPO DE TRANSPORTE </v>
       </c>
+      <c r="F32" s="7" t="s">
+        <v>166</v>
+      </c>
       <c r="H32" s="3"/>
     </row>
     <row r="33" spans="1:9" ht="15" x14ac:dyDescent="0.25">
@@ -1827,6 +1963,9 @@
         <f>TblCatalogoCuentas[[#This Row],[Código]] &amp; " - " &amp; TblCatalogoCuentas[[#This Row],[Descripción]]</f>
         <v>121002004 - EQUIPO DE SEGURIDAD</v>
       </c>
+      <c r="F33" s="7" t="s">
+        <v>166</v>
+      </c>
       <c r="H33" s="3"/>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.3">
@@ -1848,6 +1987,9 @@
         <f>TblCatalogoCuentas[[#This Row],[Código]] &amp; " - " &amp; TblCatalogoCuentas[[#This Row],[Descripción]]</f>
         <v xml:space="preserve">121003 - DEPRECIACIÓN ACUMULADA </v>
       </c>
+      <c r="F34" s="7" t="s">
+        <v>166</v>
+      </c>
       <c r="H34" s="3"/>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.3">
@@ -1869,6 +2011,9 @@
         <f>TblCatalogoCuentas[[#This Row],[Código]] &amp; " - " &amp; TblCatalogoCuentas[[#This Row],[Descripción]]</f>
         <v xml:space="preserve">121003001 - DEPRECIACIÓN ACUMULADA DE INSTALACIONES </v>
       </c>
+      <c r="F35" s="7" t="s">
+        <v>166</v>
+      </c>
       <c r="H35" s="3"/>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.3">
@@ -1890,6 +2035,9 @@
         <f>TblCatalogoCuentas[[#This Row],[Código]] &amp; " - " &amp; TblCatalogoCuentas[[#This Row],[Descripción]]</f>
         <v xml:space="preserve">121003002 - DEPRECIACIÓN ACUMULADA MOBILIARIO Y EQUIPO DE OFICINA </v>
       </c>
+      <c r="F36" s="7" t="s">
+        <v>166</v>
+      </c>
       <c r="H36" s="3"/>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.3">
@@ -1911,6 +2059,9 @@
         <f>TblCatalogoCuentas[[#This Row],[Código]] &amp; " - " &amp; TblCatalogoCuentas[[#This Row],[Descripción]]</f>
         <v>121003003 - DEPRECIACIÓN ACUMULADA MOBILIARIO Y EQUIPO DE VENTA</v>
       </c>
+      <c r="F37" s="7" t="s">
+        <v>166</v>
+      </c>
       <c r="H37" s="3"/>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.3">
@@ -1932,6 +2083,9 @@
         <f>TblCatalogoCuentas[[#This Row],[Código]] &amp; " - " &amp; TblCatalogoCuentas[[#This Row],[Descripción]]</f>
         <v xml:space="preserve">121003004 - DEPRECIACIÓN ACUMULADA EQUIPO DE TRANSPORTE </v>
       </c>
+      <c r="F38" s="7" t="s">
+        <v>166</v>
+      </c>
       <c r="H38" s="3"/>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.3">
@@ -1953,6 +2107,9 @@
         <f>TblCatalogoCuentas[[#This Row],[Código]] &amp; " - " &amp; TblCatalogoCuentas[[#This Row],[Descripción]]</f>
         <v xml:space="preserve">121003005 - DEPRECIACIÓN ACUMULADA EQUIPO DE SEGURIDAD </v>
       </c>
+      <c r="F39" s="7" t="s">
+        <v>166</v>
+      </c>
       <c r="H39" s="3"/>
     </row>
     <row r="40" spans="1:9" ht="15" x14ac:dyDescent="0.25">
@@ -1974,6 +2131,9 @@
         <f>TblCatalogoCuentas[[#This Row],[Código]] &amp; " - " &amp; TblCatalogoCuentas[[#This Row],[Descripción]]</f>
         <v xml:space="preserve">122 - INTANGIBLES </v>
       </c>
+      <c r="F40" s="7" t="s">
+        <v>166</v>
+      </c>
       <c r="I40" s="3"/>
     </row>
     <row r="41" spans="1:9" ht="15" x14ac:dyDescent="0.25">
@@ -1995,6 +2155,9 @@
         <f>TblCatalogoCuentas[[#This Row],[Código]] &amp; " - " &amp; TblCatalogoCuentas[[#This Row],[Descripción]]</f>
         <v>122001 - PATENTES Y MARCA</v>
       </c>
+      <c r="F41" s="7" t="s">
+        <v>166</v>
+      </c>
       <c r="H41" s="3"/>
     </row>
     <row r="42" spans="1:9" ht="15" x14ac:dyDescent="0.25">
@@ -2016,6 +2179,9 @@
         <f>TblCatalogoCuentas[[#This Row],[Código]] &amp; " - " &amp; TblCatalogoCuentas[[#This Row],[Descripción]]</f>
         <v>122002 - SOFTWARE</v>
       </c>
+      <c r="F42" s="7" t="s">
+        <v>166</v>
+      </c>
       <c r="H42" s="3"/>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.3">
@@ -2037,6 +2203,9 @@
         <f>TblCatalogoCuentas[[#This Row],[Código]] &amp; " - " &amp; TblCatalogoCuentas[[#This Row],[Descripción]]</f>
         <v xml:space="preserve">122003 - AMORTIZACIÓN ACUMULADA DE INTANGIBLES </v>
       </c>
+      <c r="F43" s="7" t="s">
+        <v>166</v>
+      </c>
       <c r="H43" s="3"/>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.3">
@@ -2058,6 +2227,9 @@
         <f>TblCatalogoCuentas[[#This Row],[Código]] &amp; " - " &amp; TblCatalogoCuentas[[#This Row],[Descripción]]</f>
         <v xml:space="preserve">122003001 - AMORTIZACIÓN ACUMULADA PATENTES Y MARCA </v>
       </c>
+      <c r="F44" s="7" t="s">
+        <v>166</v>
+      </c>
       <c r="H44" s="3"/>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.3">
@@ -2079,6 +2251,9 @@
         <f>TblCatalogoCuentas[[#This Row],[Código]] &amp; " - " &amp; TblCatalogoCuentas[[#This Row],[Descripción]]</f>
         <v xml:space="preserve">122003002 - AMORTIZACIÓN ACUMULADA SOFTWARE </v>
       </c>
+      <c r="F45" s="7" t="s">
+        <v>166</v>
+      </c>
       <c r="H45" s="3"/>
     </row>
     <row r="46" spans="1:9" ht="15" x14ac:dyDescent="0.25">
@@ -2100,6 +2275,9 @@
         <f>TblCatalogoCuentas[[#This Row],[Código]] &amp; " - " &amp; TblCatalogoCuentas[[#This Row],[Descripción]]</f>
         <v xml:space="preserve">123 - DEUDORES COMERCIALES Y OTRAS CUENTAS POR COBRAR A LARGO PLAZO </v>
       </c>
+      <c r="F46" s="7" t="s">
+        <v>166</v>
+      </c>
       <c r="I46" s="4"/>
     </row>
     <row r="47" spans="1:9" ht="15" x14ac:dyDescent="0.25">
@@ -2121,6 +2299,9 @@
         <f>TblCatalogoCuentas[[#This Row],[Código]] &amp; " - " &amp; TblCatalogoCuentas[[#This Row],[Descripción]]</f>
         <v>124 - INVERSIONES FINANCIERAS A LARGO PLAZO</v>
       </c>
+      <c r="F47" s="7" t="s">
+        <v>166</v>
+      </c>
       <c r="I47" s="3"/>
     </row>
     <row r="48" spans="1:9" ht="15" x14ac:dyDescent="0.25">
@@ -2142,6 +2323,9 @@
         <f>TblCatalogoCuentas[[#This Row],[Código]] &amp; " - " &amp; TblCatalogoCuentas[[#This Row],[Descripción]]</f>
         <v xml:space="preserve">2 - PASIVO </v>
       </c>
+      <c r="F48" s="7" t="s">
+        <v>167</v>
+      </c>
       <c r="I48" s="2"/>
     </row>
     <row r="49" spans="1:9" ht="15" x14ac:dyDescent="0.25">
@@ -2163,6 +2347,9 @@
         <f>TblCatalogoCuentas[[#This Row],[Código]] &amp; " - " &amp; TblCatalogoCuentas[[#This Row],[Descripción]]</f>
         <v xml:space="preserve">21 - PASIVO CORRIENTE </v>
       </c>
+      <c r="F49" s="7" t="s">
+        <v>167</v>
+      </c>
       <c r="I49" s="2"/>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.3">
@@ -2184,6 +2371,9 @@
         <f>TblCatalogoCuentas[[#This Row],[Código]] &amp; " - " &amp; TblCatalogoCuentas[[#This Row],[Descripción]]</f>
         <v>211 - PRÉSTAMOS Y SOBREGIROS BANCARIOS A CORTO PLAZO</v>
       </c>
+      <c r="F50" s="7" t="s">
+        <v>167</v>
+      </c>
       <c r="I50" s="3"/>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.3">
@@ -2205,6 +2395,9 @@
         <f>TblCatalogoCuentas[[#This Row],[Código]] &amp; " - " &amp; TblCatalogoCuentas[[#This Row],[Descripción]]</f>
         <v xml:space="preserve">212 - PORCIÓN CORRIENTE DE PRESTAMOS A LARGO PLAZO </v>
       </c>
+      <c r="F51" s="7" t="s">
+        <v>167</v>
+      </c>
       <c r="I51" s="3"/>
     </row>
     <row r="52" spans="1:9" ht="15" x14ac:dyDescent="0.25">
@@ -2226,6 +2419,9 @@
         <f>TblCatalogoCuentas[[#This Row],[Código]] &amp; " - " &amp; TblCatalogoCuentas[[#This Row],[Descripción]]</f>
         <v xml:space="preserve">213 - ACREEDORES COMERCIALES Y OTRAS CUENTAS POR PAGAR </v>
       </c>
+      <c r="F52" s="7" t="s">
+        <v>167</v>
+      </c>
       <c r="I52" s="3"/>
     </row>
     <row r="53" spans="1:9" ht="15" x14ac:dyDescent="0.25">
@@ -2247,6 +2443,9 @@
         <f>TblCatalogoCuentas[[#This Row],[Código]] &amp; " - " &amp; TblCatalogoCuentas[[#This Row],[Descripción]]</f>
         <v>213001 - PROVEEDORES LOCALES</v>
       </c>
+      <c r="F53" s="7" t="s">
+        <v>167</v>
+      </c>
       <c r="H53" s="3"/>
     </row>
     <row r="54" spans="1:9" ht="15" x14ac:dyDescent="0.25">
@@ -2268,6 +2467,9 @@
         <f>TblCatalogoCuentas[[#This Row],[Código]] &amp; " - " &amp; TblCatalogoCuentas[[#This Row],[Descripción]]</f>
         <v>213002 - DOCUMENTOS POR PAGAR</v>
       </c>
+      <c r="F54" s="7" t="s">
+        <v>167</v>
+      </c>
       <c r="H54" s="3"/>
     </row>
     <row r="55" spans="1:9" ht="15" x14ac:dyDescent="0.25">
@@ -2289,6 +2491,9 @@
         <f>TblCatalogoCuentas[[#This Row],[Código]] &amp; " - " &amp; TblCatalogoCuentas[[#This Row],[Descripción]]</f>
         <v xml:space="preserve">213003 - INTERESES POR PAGAR </v>
       </c>
+      <c r="F55" s="7" t="s">
+        <v>167</v>
+      </c>
       <c r="H55" s="3"/>
     </row>
     <row r="56" spans="1:9" ht="15" x14ac:dyDescent="0.25">
@@ -2310,6 +2515,9 @@
         <f>TblCatalogoCuentas[[#This Row],[Código]] &amp; " - " &amp; TblCatalogoCuentas[[#This Row],[Descripción]]</f>
         <v>214 - RETENCIONES LEGALES Y OTROS ACREEDORES POR PAGAR</v>
       </c>
+      <c r="F56" s="7" t="s">
+        <v>167</v>
+      </c>
       <c r="I56" s="3"/>
     </row>
     <row r="57" spans="1:9" ht="15" x14ac:dyDescent="0.25">
@@ -2331,6 +2539,9 @@
         <f>TblCatalogoCuentas[[#This Row],[Código]] &amp; " - " &amp; TblCatalogoCuentas[[#This Row],[Descripción]]</f>
         <v>214001 - ISSS- SALUD</v>
       </c>
+      <c r="F57" s="7" t="s">
+        <v>167</v>
+      </c>
       <c r="H57" s="3"/>
     </row>
     <row r="58" spans="1:9" ht="15" x14ac:dyDescent="0.25">
@@ -2352,6 +2563,9 @@
         <f>TblCatalogoCuentas[[#This Row],[Código]] &amp; " - " &amp; TblCatalogoCuentas[[#This Row],[Descripción]]</f>
         <v>214002 - UNIDAD DE PENSIONES ISSS</v>
       </c>
+      <c r="F58" s="7" t="s">
+        <v>167</v>
+      </c>
       <c r="H58" s="3"/>
     </row>
     <row r="59" spans="1:9" ht="15" x14ac:dyDescent="0.25">
@@ -2373,6 +2587,9 @@
         <f>TblCatalogoCuentas[[#This Row],[Código]] &amp; " - " &amp; TblCatalogoCuentas[[#This Row],[Descripción]]</f>
         <v>214003 - IMPUESTO SOBRE LA RENTA EMPLEADOS PERMANENTES</v>
       </c>
+      <c r="F59" s="7" t="s">
+        <v>167</v>
+      </c>
       <c r="H59" s="3"/>
     </row>
     <row r="60" spans="1:9" ht="15" x14ac:dyDescent="0.25">
@@ -2394,6 +2611,9 @@
         <f>TblCatalogoCuentas[[#This Row],[Código]] &amp; " - " &amp; TblCatalogoCuentas[[#This Row],[Descripción]]</f>
         <v xml:space="preserve">214004 - IMPUESTO SOBRE LA RENTA SERVICIOS </v>
       </c>
+      <c r="F60" s="7" t="s">
+        <v>167</v>
+      </c>
       <c r="H60" s="3"/>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.3">
@@ -2415,6 +2635,9 @@
         <f>TblCatalogoCuentas[[#This Row],[Código]] &amp; " - " &amp; TblCatalogoCuentas[[#This Row],[Descripción]]</f>
         <v xml:space="preserve">214005 - AFP CONFÍA </v>
       </c>
+      <c r="F61" s="7" t="s">
+        <v>167</v>
+      </c>
       <c r="H61" s="3"/>
     </row>
     <row r="62" spans="1:9" ht="15" x14ac:dyDescent="0.25">
@@ -2436,6 +2659,9 @@
         <f>TblCatalogoCuentas[[#This Row],[Código]] &amp; " - " &amp; TblCatalogoCuentas[[#This Row],[Descripción]]</f>
         <v>214006 - AFP CRECER</v>
       </c>
+      <c r="F62" s="7" t="s">
+        <v>167</v>
+      </c>
       <c r="H62" s="3"/>
     </row>
     <row r="63" spans="1:9" ht="15" x14ac:dyDescent="0.25">
@@ -2457,6 +2683,9 @@
         <f>TblCatalogoCuentas[[#This Row],[Código]] &amp; " - " &amp; TblCatalogoCuentas[[#This Row],[Descripción]]</f>
         <v>215 - OBLIGACIONES POR BENEFICIOS A EMPLEADOS</v>
       </c>
+      <c r="F63" s="7" t="s">
+        <v>167</v>
+      </c>
       <c r="I63" s="3"/>
     </row>
     <row r="64" spans="1:9" ht="15" x14ac:dyDescent="0.25">
@@ -2478,6 +2707,9 @@
         <f>TblCatalogoCuentas[[#This Row],[Código]] &amp; " - " &amp; TblCatalogoCuentas[[#This Row],[Descripción]]</f>
         <v xml:space="preserve">215001 - SUELDOS </v>
       </c>
+      <c r="F64" s="7" t="s">
+        <v>167</v>
+      </c>
       <c r="H64" s="3"/>
     </row>
     <row r="65" spans="1:9" ht="15" x14ac:dyDescent="0.25">
@@ -2499,6 +2731,9 @@
         <f>TblCatalogoCuentas[[#This Row],[Código]] &amp; " - " &amp; TblCatalogoCuentas[[#This Row],[Descripción]]</f>
         <v xml:space="preserve">215002 - VACACIONES </v>
       </c>
+      <c r="F65" s="7" t="s">
+        <v>167</v>
+      </c>
       <c r="H65" s="3"/>
     </row>
     <row r="66" spans="1:9" ht="15" x14ac:dyDescent="0.25">
@@ -2520,6 +2755,9 @@
         <f>TblCatalogoCuentas[[#This Row],[Código]] &amp; " - " &amp; TblCatalogoCuentas[[#This Row],[Descripción]]</f>
         <v>215003 - AGUINALDOS</v>
       </c>
+      <c r="F66" s="7" t="s">
+        <v>167</v>
+      </c>
       <c r="H66" s="3"/>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.3">
@@ -2541,6 +2779,9 @@
         <f>TblCatalogoCuentas[[#This Row],[Código]] &amp; " - " &amp; TblCatalogoCuentas[[#This Row],[Descripción]]</f>
         <v>215004 - VIÁTICOS</v>
       </c>
+      <c r="F67" s="7" t="s">
+        <v>167</v>
+      </c>
       <c r="H67" s="3"/>
     </row>
     <row r="68" spans="1:9" ht="15" x14ac:dyDescent="0.25">
@@ -2562,6 +2803,9 @@
         <f>TblCatalogoCuentas[[#This Row],[Código]] &amp; " - " &amp; TblCatalogoCuentas[[#This Row],[Descripción]]</f>
         <v xml:space="preserve">215005 - INDEMNIZACIONES </v>
       </c>
+      <c r="F68" s="7" t="s">
+        <v>167</v>
+      </c>
       <c r="H68" s="3"/>
     </row>
     <row r="69" spans="1:9" ht="15" x14ac:dyDescent="0.25">
@@ -2583,6 +2827,9 @@
         <f>TblCatalogoCuentas[[#This Row],[Código]] &amp; " - " &amp; TblCatalogoCuentas[[#This Row],[Descripción]]</f>
         <v xml:space="preserve">215006 - COMISIONES POR VENTAS </v>
       </c>
+      <c r="F69" s="7" t="s">
+        <v>167</v>
+      </c>
       <c r="H69" s="3"/>
     </row>
     <row r="70" spans="1:9" ht="15" x14ac:dyDescent="0.25">
@@ -2604,6 +2851,9 @@
         <f>TblCatalogoCuentas[[#This Row],[Código]] &amp; " - " &amp; TblCatalogoCuentas[[#This Row],[Descripción]]</f>
         <v xml:space="preserve">215007 - BONIFICACIONES </v>
       </c>
+      <c r="F70" s="7" t="s">
+        <v>167</v>
+      </c>
       <c r="H70" s="3"/>
     </row>
     <row r="71" spans="1:9" ht="15" x14ac:dyDescent="0.25">
@@ -2625,6 +2875,9 @@
         <f>TblCatalogoCuentas[[#This Row],[Código]] &amp; " - " &amp; TblCatalogoCuentas[[#This Row],[Descripción]]</f>
         <v xml:space="preserve">216 - IMPUESTOS POR PAGAR </v>
       </c>
+      <c r="F71" s="7" t="s">
+        <v>167</v>
+      </c>
       <c r="I71" s="3"/>
     </row>
     <row r="72" spans="1:9" ht="15" x14ac:dyDescent="0.25">
@@ -2646,6 +2899,9 @@
         <f>TblCatalogoCuentas[[#This Row],[Código]] &amp; " - " &amp; TblCatalogoCuentas[[#This Row],[Descripción]]</f>
         <v>216001 - IVA POR PAGAR</v>
       </c>
+      <c r="F72" s="7" t="s">
+        <v>167</v>
+      </c>
       <c r="H72" s="3"/>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.3">
@@ -2667,6 +2923,9 @@
         <f>TblCatalogoCuentas[[#This Row],[Código]] &amp; " - " &amp; TblCatalogoCuentas[[#This Row],[Descripción]]</f>
         <v xml:space="preserve">217 - IVA DÉBITO FISCAL </v>
       </c>
+      <c r="F73" s="7" t="s">
+        <v>167</v>
+      </c>
       <c r="I73" s="3"/>
     </row>
     <row r="74" spans="1:9" ht="15" x14ac:dyDescent="0.25">
@@ -2688,6 +2947,9 @@
         <f>TblCatalogoCuentas[[#This Row],[Código]] &amp; " - " &amp; TblCatalogoCuentas[[#This Row],[Descripción]]</f>
         <v>217003 - CONSUMIDORES FINALES</v>
       </c>
+      <c r="F74" s="7" t="s">
+        <v>167</v>
+      </c>
       <c r="H74" s="3"/>
     </row>
     <row r="75" spans="1:9" ht="15" x14ac:dyDescent="0.25">
@@ -2709,6 +2971,9 @@
         <f>TblCatalogoCuentas[[#This Row],[Código]] &amp; " - " &amp; TblCatalogoCuentas[[#This Row],[Descripción]]</f>
         <v>218 - ASUNTOS PENDIENTES</v>
       </c>
+      <c r="F75" s="7" t="s">
+        <v>167</v>
+      </c>
       <c r="I75" s="3"/>
     </row>
     <row r="76" spans="1:9" ht="15" x14ac:dyDescent="0.25">
@@ -2730,6 +2995,9 @@
         <f>TblCatalogoCuentas[[#This Row],[Código]] &amp; " - " &amp; TblCatalogoCuentas[[#This Row],[Descripción]]</f>
         <v xml:space="preserve">218001 - SOBRANTES DE CAJA </v>
       </c>
+      <c r="F76" s="7" t="s">
+        <v>167</v>
+      </c>
       <c r="H76" s="3"/>
     </row>
     <row r="77" spans="1:9" ht="15" x14ac:dyDescent="0.25">
@@ -2751,6 +3019,9 @@
         <f>TblCatalogoCuentas[[#This Row],[Código]] &amp; " - " &amp; TblCatalogoCuentas[[#This Row],[Descripción]]</f>
         <v xml:space="preserve">219 - ANTICIPOS DE CLIENTES </v>
       </c>
+      <c r="F77" s="7" t="s">
+        <v>167</v>
+      </c>
       <c r="I77" s="3"/>
     </row>
     <row r="78" spans="1:9" ht="15" x14ac:dyDescent="0.25">
@@ -2772,6 +3043,9 @@
         <f>TblCatalogoCuentas[[#This Row],[Código]] &amp; " - " &amp; TblCatalogoCuentas[[#This Row],[Descripción]]</f>
         <v xml:space="preserve">219001 - REBAJAS Y DEVOLUCIONES PENDIENTES DE APLICAR </v>
       </c>
+      <c r="F78" s="7" t="s">
+        <v>167</v>
+      </c>
       <c r="H78" s="3"/>
     </row>
     <row r="79" spans="1:9" ht="15" x14ac:dyDescent="0.25">
@@ -2793,6 +3067,9 @@
         <f>TblCatalogoCuentas[[#This Row],[Código]] &amp; " - " &amp; TblCatalogoCuentas[[#This Row],[Descripción]]</f>
         <v xml:space="preserve">22 - PASIVO NO CORRIENTE </v>
       </c>
+      <c r="F79" s="7" t="s">
+        <v>167</v>
+      </c>
       <c r="I79" s="2"/>
     </row>
     <row r="80" spans="1:9" ht="15" x14ac:dyDescent="0.25">
@@ -2814,6 +3091,9 @@
         <f>TblCatalogoCuentas[[#This Row],[Código]] &amp; " - " &amp; TblCatalogoCuentas[[#This Row],[Descripción]]</f>
         <v xml:space="preserve">221 - PASIVO POR IMPUESTOS DIFERIDOS </v>
       </c>
+      <c r="F80" s="7" t="s">
+        <v>167</v>
+      </c>
       <c r="I80" s="3"/>
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.3">
@@ -2835,6 +3115,9 @@
         <f>TblCatalogoCuentas[[#This Row],[Código]] &amp; " - " &amp; TblCatalogoCuentas[[#This Row],[Descripción]]</f>
         <v xml:space="preserve">222 - PRÉSTAMOS BANCARIOS A LARGO PLAZO </v>
       </c>
+      <c r="F81" s="7" t="s">
+        <v>167</v>
+      </c>
       <c r="I81" s="3"/>
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.3">
@@ -2856,6 +3139,9 @@
         <f>TblCatalogoCuentas[[#This Row],[Código]] &amp; " - " &amp; TblCatalogoCuentas[[#This Row],[Descripción]]</f>
         <v xml:space="preserve">222001 - GARANTÍA HIPOTECARIA  </v>
       </c>
+      <c r="F82" s="7" t="s">
+        <v>167</v>
+      </c>
       <c r="H82" s="3"/>
     </row>
     <row r="83" spans="1:9" ht="15" x14ac:dyDescent="0.25">
@@ -2877,6 +3163,7 @@
         <f>TblCatalogoCuentas[[#This Row],[Código]] &amp; " - " &amp; TblCatalogoCuentas[[#This Row],[Descripción]]</f>
         <v xml:space="preserve">3 - PATRIMONIO </v>
       </c>
+      <c r="F83" s="7"/>
       <c r="I83" s="2"/>
     </row>
     <row r="84" spans="1:9" ht="15" x14ac:dyDescent="0.25">
@@ -2898,6 +3185,7 @@
         <f>TblCatalogoCuentas[[#This Row],[Código]] &amp; " - " &amp; TblCatalogoCuentas[[#This Row],[Descripción]]</f>
         <v xml:space="preserve">31 - CAPITAL CONTABLE </v>
       </c>
+      <c r="F84" s="7"/>
       <c r="I84" s="2"/>
     </row>
     <row r="85" spans="1:9" ht="15" x14ac:dyDescent="0.25">
@@ -2919,6 +3207,7 @@
         <f>TblCatalogoCuentas[[#This Row],[Código]] &amp; " - " &amp; TblCatalogoCuentas[[#This Row],[Descripción]]</f>
         <v xml:space="preserve">311 - CAPITAL </v>
       </c>
+      <c r="F85" s="7"/>
       <c r="I85" s="3"/>
     </row>
     <row r="86" spans="1:9" ht="15" x14ac:dyDescent="0.25">
@@ -2940,6 +3229,7 @@
         <f>TblCatalogoCuentas[[#This Row],[Código]] &amp; " - " &amp; TblCatalogoCuentas[[#This Row],[Descripción]]</f>
         <v xml:space="preserve">312 - RESULTADO DEL EJERCICIO </v>
       </c>
+      <c r="F86" s="7"/>
       <c r="I86" s="3"/>
     </row>
     <row r="87" spans="1:9" ht="15" x14ac:dyDescent="0.25">
@@ -2961,6 +3251,7 @@
         <f>TblCatalogoCuentas[[#This Row],[Código]] &amp; " - " &amp; TblCatalogoCuentas[[#This Row],[Descripción]]</f>
         <v xml:space="preserve">312001 - UTILIDAD DEL PRESENTE EJERCICIO </v>
       </c>
+      <c r="F87" s="7"/>
       <c r="H87" s="3"/>
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.3">
@@ -2982,6 +3273,7 @@
         <f>TblCatalogoCuentas[[#This Row],[Código]] &amp; " - " &amp; TblCatalogoCuentas[[#This Row],[Descripción]]</f>
         <v xml:space="preserve">312002 - PÉRDIDA DEL PRESENTE EJERCICIO </v>
       </c>
+      <c r="F88" s="7"/>
       <c r="H88" s="3"/>
     </row>
     <row r="89" spans="1:9" ht="15" x14ac:dyDescent="0.25">
@@ -3003,6 +3295,7 @@
         <f>TblCatalogoCuentas[[#This Row],[Código]] &amp; " - " &amp; TblCatalogoCuentas[[#This Row],[Descripción]]</f>
         <v xml:space="preserve">4 - CUENTAS DE RESULTADO DEUDORAS </v>
       </c>
+      <c r="F89" s="7"/>
       <c r="I89" s="2"/>
     </row>
     <row r="90" spans="1:9" ht="15" x14ac:dyDescent="0.25">
@@ -3024,6 +3317,7 @@
         <f>TblCatalogoCuentas[[#This Row],[Código]] &amp; " - " &amp; TblCatalogoCuentas[[#This Row],[Descripción]]</f>
         <v xml:space="preserve">41 - COMPRAS Y COSTOS </v>
       </c>
+      <c r="F90" s="7"/>
       <c r="I90" s="2"/>
     </row>
     <row r="91" spans="1:9" ht="15" x14ac:dyDescent="0.25">
@@ -3045,6 +3339,7 @@
         <f>TblCatalogoCuentas[[#This Row],[Código]] &amp; " - " &amp; TblCatalogoCuentas[[#This Row],[Descripción]]</f>
         <v xml:space="preserve">411 - COMPRAS </v>
       </c>
+      <c r="F91" s="7"/>
       <c r="I91" s="3"/>
     </row>
     <row r="92" spans="1:9" ht="15" x14ac:dyDescent="0.25">
@@ -3066,6 +3361,7 @@
         <f>TblCatalogoCuentas[[#This Row],[Código]] &amp; " - " &amp; TblCatalogoCuentas[[#This Row],[Descripción]]</f>
         <v>411001 - COMPRAS AL CONTADO</v>
       </c>
+      <c r="F92" s="7"/>
       <c r="H92" s="3"/>
     </row>
     <row r="93" spans="1:9" x14ac:dyDescent="0.3">
@@ -3087,6 +3383,7 @@
         <f>TblCatalogoCuentas[[#This Row],[Código]] &amp; " - " &amp; TblCatalogoCuentas[[#This Row],[Descripción]]</f>
         <v>411002 - COMPRAS AL CRÉDITO</v>
       </c>
+      <c r="F93" s="7"/>
       <c r="H93" s="3"/>
     </row>
     <row r="94" spans="1:9" ht="15" x14ac:dyDescent="0.25">
@@ -3108,6 +3405,7 @@
         <f>TblCatalogoCuentas[[#This Row],[Código]] &amp; " - " &amp; TblCatalogoCuentas[[#This Row],[Descripción]]</f>
         <v xml:space="preserve">412 - GASTOS SOBRE COMPRAS </v>
       </c>
+      <c r="F94" s="7"/>
       <c r="I94" s="3"/>
     </row>
     <row r="95" spans="1:9" ht="15" x14ac:dyDescent="0.25">
@@ -3129,6 +3427,7 @@
         <f>TblCatalogoCuentas[[#This Row],[Código]] &amp; " - " &amp; TblCatalogoCuentas[[#This Row],[Descripción]]</f>
         <v>413 - REBAJAS, DEVOLUCIONES SOBRE VENTAS</v>
       </c>
+      <c r="F95" s="7"/>
       <c r="I95" s="3"/>
     </row>
     <row r="96" spans="1:9" ht="15" x14ac:dyDescent="0.25">
@@ -3150,6 +3449,7 @@
         <f>TblCatalogoCuentas[[#This Row],[Código]] &amp; " - " &amp; TblCatalogoCuentas[[#This Row],[Descripción]]</f>
         <v>413001 - REBAJAS Y DEVOLUCIONES SOBRE VENTAS AL CONTADO</v>
       </c>
+      <c r="F96" s="7"/>
       <c r="H96" s="3"/>
     </row>
     <row r="97" spans="1:9" x14ac:dyDescent="0.3">
@@ -3171,6 +3471,7 @@
         <f>TblCatalogoCuentas[[#This Row],[Código]] &amp; " - " &amp; TblCatalogoCuentas[[#This Row],[Descripción]]</f>
         <v xml:space="preserve">413002 - REBAJAS Y DEVOLUCIONES SOBRE VENTAS AL CRÉDITO </v>
       </c>
+      <c r="F97" s="7"/>
       <c r="H97" s="3"/>
     </row>
     <row r="98" spans="1:9" ht="15" x14ac:dyDescent="0.25">
@@ -3192,6 +3493,7 @@
         <f>TblCatalogoCuentas[[#This Row],[Código]] &amp; " - " &amp; TblCatalogoCuentas[[#This Row],[Descripción]]</f>
         <v xml:space="preserve">414 - COSTO DE VENTA </v>
       </c>
+      <c r="F98" s="7"/>
       <c r="I98" s="3"/>
     </row>
     <row r="99" spans="1:9" x14ac:dyDescent="0.3">
@@ -3213,6 +3515,7 @@
         <f>TblCatalogoCuentas[[#This Row],[Código]] &amp; " - " &amp; TblCatalogoCuentas[[#This Row],[Descripción]]</f>
         <v>414001 - COSTO DE VENTA DE MERCANCÍAS</v>
       </c>
+      <c r="F99" s="7"/>
       <c r="H99" s="3"/>
     </row>
     <row r="100" spans="1:9" x14ac:dyDescent="0.3">
@@ -3234,6 +3537,7 @@
         <f>TblCatalogoCuentas[[#This Row],[Código]] &amp; " - " &amp; TblCatalogoCuentas[[#This Row],[Descripción]]</f>
         <v xml:space="preserve">42 - GASTOS DE OPERACIÓN </v>
       </c>
+      <c r="F100" s="7"/>
       <c r="I100" s="2"/>
     </row>
     <row r="101" spans="1:9" x14ac:dyDescent="0.3">
@@ -3255,6 +3559,7 @@
         <f>TblCatalogoCuentas[[#This Row],[Código]] &amp; " - " &amp; TblCatalogoCuentas[[#This Row],[Descripción]]</f>
         <v xml:space="preserve">421 - GASTOS DE ADMINISTRACIÓN </v>
       </c>
+      <c r="F101" s="7"/>
       <c r="I101" s="3"/>
     </row>
     <row r="102" spans="1:9" ht="15" x14ac:dyDescent="0.25">
@@ -3276,6 +3581,7 @@
         <f>TblCatalogoCuentas[[#This Row],[Código]] &amp; " - " &amp; TblCatalogoCuentas[[#This Row],[Descripción]]</f>
         <v>421001 - SUELDOS</v>
       </c>
+      <c r="F102" s="7"/>
       <c r="H102" s="3"/>
     </row>
     <row r="103" spans="1:9" ht="15" x14ac:dyDescent="0.25">
@@ -3297,6 +3603,7 @@
         <f>TblCatalogoCuentas[[#This Row],[Código]] &amp; " - " &amp; TblCatalogoCuentas[[#This Row],[Descripción]]</f>
         <v>421002 - VACACIONES Y BONIFICACIONES</v>
       </c>
+      <c r="F103" s="7"/>
       <c r="H103" s="3"/>
     </row>
     <row r="104" spans="1:9" ht="15" x14ac:dyDescent="0.25">
@@ -3318,6 +3625,7 @@
         <f>TblCatalogoCuentas[[#This Row],[Código]] &amp; " - " &amp; TblCatalogoCuentas[[#This Row],[Descripción]]</f>
         <v xml:space="preserve">421003 - AGUINALDOS Y GRATIFICACIONES </v>
       </c>
+      <c r="F104" s="7"/>
       <c r="H104" s="3"/>
     </row>
     <row r="105" spans="1:9" ht="15" x14ac:dyDescent="0.25">
@@ -3339,6 +3647,7 @@
         <f>TblCatalogoCuentas[[#This Row],[Código]] &amp; " - " &amp; TblCatalogoCuentas[[#This Row],[Descripción]]</f>
         <v xml:space="preserve">421004 - SEGURO SOCIAL </v>
       </c>
+      <c r="F105" s="7"/>
       <c r="H105" s="3"/>
     </row>
     <row r="106" spans="1:9" x14ac:dyDescent="0.3">
@@ -3360,6 +3669,7 @@
         <f>TblCatalogoCuentas[[#This Row],[Código]] &amp; " - " &amp; TblCatalogoCuentas[[#This Row],[Descripción]]</f>
         <v xml:space="preserve">421005 - PAPELERÍA Y ÚTILES </v>
       </c>
+      <c r="F106" s="7"/>
       <c r="H106" s="3"/>
     </row>
     <row r="107" spans="1:9" ht="15" x14ac:dyDescent="0.25">
@@ -3381,6 +3691,7 @@
         <f>TblCatalogoCuentas[[#This Row],[Código]] &amp; " - " &amp; TblCatalogoCuentas[[#This Row],[Descripción]]</f>
         <v>421006 - IMPUESTOS</v>
       </c>
+      <c r="F107" s="7"/>
       <c r="H107" s="3"/>
     </row>
     <row r="108" spans="1:9" x14ac:dyDescent="0.3">
@@ -3402,6 +3713,7 @@
         <f>TblCatalogoCuentas[[#This Row],[Código]] &amp; " - " &amp; TblCatalogoCuentas[[#This Row],[Descripción]]</f>
         <v xml:space="preserve">421007 - LUZ ELÉCTRICA </v>
       </c>
+      <c r="F108" s="7"/>
       <c r="H108" s="3"/>
     </row>
     <row r="109" spans="1:9" ht="15" x14ac:dyDescent="0.25">
@@ -3423,6 +3735,7 @@
         <f>TblCatalogoCuentas[[#This Row],[Código]] &amp; " - " &amp; TblCatalogoCuentas[[#This Row],[Descripción]]</f>
         <v xml:space="preserve">422 - GASTOS DE VENTA </v>
       </c>
+      <c r="F109" s="7"/>
       <c r="I109" s="3"/>
     </row>
     <row r="110" spans="1:9" ht="15" x14ac:dyDescent="0.25">
@@ -3444,6 +3757,7 @@
         <f>TblCatalogoCuentas[[#This Row],[Código]] &amp; " - " &amp; TblCatalogoCuentas[[#This Row],[Descripción]]</f>
         <v>422001 - SUELDOS</v>
       </c>
+      <c r="F110" s="7"/>
       <c r="H110" s="3"/>
     </row>
     <row r="111" spans="1:9" ht="15" x14ac:dyDescent="0.25">
@@ -3465,6 +3779,7 @@
         <f>TblCatalogoCuentas[[#This Row],[Código]] &amp; " - " &amp; TblCatalogoCuentas[[#This Row],[Descripción]]</f>
         <v>422002 - VACACIONES Y BONIFICACIONES</v>
       </c>
+      <c r="F111" s="7"/>
       <c r="H111" s="3"/>
     </row>
     <row r="112" spans="1:9" ht="15" x14ac:dyDescent="0.25">
@@ -3486,6 +3801,7 @@
         <f>TblCatalogoCuentas[[#This Row],[Código]] &amp; " - " &amp; TblCatalogoCuentas[[#This Row],[Descripción]]</f>
         <v xml:space="preserve">422003 - AGUINALDOS Y GRATIFICACIONES </v>
       </c>
+      <c r="F112" s="7"/>
       <c r="H112" s="3"/>
     </row>
     <row r="113" spans="1:9" ht="15" x14ac:dyDescent="0.25">
@@ -3507,6 +3823,7 @@
         <f>TblCatalogoCuentas[[#This Row],[Código]] &amp; " - " &amp; TblCatalogoCuentas[[#This Row],[Descripción]]</f>
         <v xml:space="preserve">422004 - SEGURO SOCIAL </v>
       </c>
+      <c r="F113" s="7"/>
       <c r="H113" s="3"/>
     </row>
     <row r="114" spans="1:9" x14ac:dyDescent="0.3">
@@ -3528,6 +3845,7 @@
         <f>TblCatalogoCuentas[[#This Row],[Código]] &amp; " - " &amp; TblCatalogoCuentas[[#This Row],[Descripción]]</f>
         <v xml:space="preserve">422005 - PAPELERÍA Y ÚTILES </v>
       </c>
+      <c r="F114" s="7"/>
       <c r="H114" s="3"/>
     </row>
     <row r="115" spans="1:9" ht="15" x14ac:dyDescent="0.25">
@@ -3549,6 +3867,7 @@
         <f>TblCatalogoCuentas[[#This Row],[Código]] &amp; " - " &amp; TblCatalogoCuentas[[#This Row],[Descripción]]</f>
         <v>422006 - IMPUESTOS</v>
       </c>
+      <c r="F115" s="7"/>
       <c r="H115" s="3"/>
     </row>
     <row r="116" spans="1:9" x14ac:dyDescent="0.3">
@@ -3570,6 +3889,7 @@
         <f>TblCatalogoCuentas[[#This Row],[Código]] &amp; " - " &amp; TblCatalogoCuentas[[#This Row],[Descripción]]</f>
         <v xml:space="preserve">422007 - LUZ ELÉCTRICA </v>
       </c>
+      <c r="F116" s="7"/>
       <c r="H116" s="3"/>
     </row>
     <row r="117" spans="1:9" ht="15" x14ac:dyDescent="0.25">
@@ -3591,6 +3911,7 @@
         <f>TblCatalogoCuentas[[#This Row],[Código]] &amp; " - " &amp; TblCatalogoCuentas[[#This Row],[Descripción]]</f>
         <v xml:space="preserve">423 - GASTOS FINANCIEROS </v>
       </c>
+      <c r="F117" s="7"/>
       <c r="I117" s="3"/>
     </row>
     <row r="118" spans="1:9" ht="15" x14ac:dyDescent="0.25">
@@ -3612,6 +3933,7 @@
         <f>TblCatalogoCuentas[[#This Row],[Código]] &amp; " - " &amp; TblCatalogoCuentas[[#This Row],[Descripción]]</f>
         <v>423001 - INTERESES</v>
       </c>
+      <c r="F118" s="7"/>
       <c r="H118" s="3"/>
     </row>
     <row r="119" spans="1:9" ht="15" x14ac:dyDescent="0.25">
@@ -3633,6 +3955,7 @@
         <f>TblCatalogoCuentas[[#This Row],[Código]] &amp; " - " &amp; TblCatalogoCuentas[[#This Row],[Descripción]]</f>
         <v xml:space="preserve">423002 - BONIFICACIONES A CLIENTES </v>
       </c>
+      <c r="F119" s="7"/>
       <c r="H119" s="3"/>
     </row>
     <row r="120" spans="1:9" ht="15" x14ac:dyDescent="0.25">
@@ -3654,6 +3977,7 @@
         <f>TblCatalogoCuentas[[#This Row],[Código]] &amp; " - " &amp; TblCatalogoCuentas[[#This Row],[Descripción]]</f>
         <v>423003 - OTROS</v>
       </c>
+      <c r="F120" s="7"/>
       <c r="H120" s="3"/>
     </row>
     <row r="121" spans="1:9" ht="15" x14ac:dyDescent="0.25">
@@ -3675,6 +3999,7 @@
         <f>TblCatalogoCuentas[[#This Row],[Código]] &amp; " - " &amp; TblCatalogoCuentas[[#This Row],[Descripción]]</f>
         <v xml:space="preserve">424 - OTROS GASTOS NO OPERACIONALES </v>
       </c>
+      <c r="F121" s="7"/>
       <c r="I121" s="3"/>
     </row>
     <row r="122" spans="1:9" x14ac:dyDescent="0.3">
@@ -3696,6 +4021,7 @@
         <f>TblCatalogoCuentas[[#This Row],[Código]] &amp; " - " &amp; TblCatalogoCuentas[[#This Row],[Descripción]]</f>
         <v xml:space="preserve">424001 - PÉRDIDA DE CAPITAL </v>
       </c>
+      <c r="F122" s="7"/>
       <c r="H122" s="3"/>
     </row>
     <row r="123" spans="1:9" x14ac:dyDescent="0.3">
@@ -3717,6 +4043,7 @@
         <f>TblCatalogoCuentas[[#This Row],[Código]] &amp; " - " &amp; TblCatalogoCuentas[[#This Row],[Descripción]]</f>
         <v xml:space="preserve">424002 - PÉRDIDA DE INVERSIONES </v>
       </c>
+      <c r="F123" s="7"/>
       <c r="H123" s="3"/>
     </row>
     <row r="124" spans="1:9" x14ac:dyDescent="0.3">
@@ -3738,6 +4065,7 @@
         <f>TblCatalogoCuentas[[#This Row],[Código]] &amp; " - " &amp; TblCatalogoCuentas[[#This Row],[Descripción]]</f>
         <v xml:space="preserve">424003 - PÉRDIDA EN INVENTARIOS </v>
       </c>
+      <c r="F124" s="7"/>
       <c r="H124" s="3"/>
     </row>
     <row r="125" spans="1:9" x14ac:dyDescent="0.3">
@@ -3759,6 +4087,7 @@
         <f>TblCatalogoCuentas[[#This Row],[Código]] &amp; " - " &amp; TblCatalogoCuentas[[#This Row],[Descripción]]</f>
         <v xml:space="preserve">424004 - PÉRDIDA EN VENTA DE ACTIVO FIJO </v>
       </c>
+      <c r="F125" s="7"/>
       <c r="H125" s="3"/>
     </row>
     <row r="126" spans="1:9" ht="15" x14ac:dyDescent="0.25">
@@ -3780,6 +4109,7 @@
         <f>TblCatalogoCuentas[[#This Row],[Código]] &amp; " - " &amp; TblCatalogoCuentas[[#This Row],[Descripción]]</f>
         <v xml:space="preserve">43 - GASTO POR IMPUESTO SOBRE LAS GANACIAS </v>
       </c>
+      <c r="F126" s="7"/>
       <c r="I126" s="2"/>
     </row>
     <row r="127" spans="1:9" ht="15" x14ac:dyDescent="0.25">
@@ -3801,6 +4131,7 @@
         <f>TblCatalogoCuentas[[#This Row],[Código]] &amp; " - " &amp; TblCatalogoCuentas[[#This Row],[Descripción]]</f>
         <v xml:space="preserve">431 - GASTOS DE IMPUESTOS SOBRE LA RENTA </v>
       </c>
+      <c r="F127" s="7"/>
       <c r="I127" s="3"/>
     </row>
     <row r="128" spans="1:9" ht="15" x14ac:dyDescent="0.25">
@@ -3822,6 +4153,7 @@
         <f>TblCatalogoCuentas[[#This Row],[Código]] &amp; " - " &amp; TblCatalogoCuentas[[#This Row],[Descripción]]</f>
         <v xml:space="preserve">431001 - GASTO DE IMPUESTO SOBRE LA RENTA CORRIENTE </v>
       </c>
+      <c r="F128" s="7"/>
       <c r="H128" s="3"/>
     </row>
     <row r="129" spans="1:9" ht="15" x14ac:dyDescent="0.25">
@@ -3843,6 +4175,7 @@
         <f>TblCatalogoCuentas[[#This Row],[Código]] &amp; " - " &amp; TblCatalogoCuentas[[#This Row],[Descripción]]</f>
         <v xml:space="preserve">5 - CUENTAS DE RESULTADO ACREEDORAS </v>
       </c>
+      <c r="F129" s="7"/>
       <c r="I129" s="2"/>
     </row>
     <row r="130" spans="1:9" x14ac:dyDescent="0.3">
@@ -3864,6 +4197,7 @@
         <f>TblCatalogoCuentas[[#This Row],[Código]] &amp; " - " &amp; TblCatalogoCuentas[[#This Row],[Descripción]]</f>
         <v xml:space="preserve">51 - INGRESOS DE OPERACIÓN </v>
       </c>
+      <c r="F130" s="7"/>
       <c r="I130" s="2"/>
     </row>
     <row r="131" spans="1:9" ht="15" x14ac:dyDescent="0.25">
@@ -3885,6 +4219,7 @@
         <f>TblCatalogoCuentas[[#This Row],[Código]] &amp; " - " &amp; TblCatalogoCuentas[[#This Row],[Descripción]]</f>
         <v xml:space="preserve">511 - VENTAS </v>
       </c>
+      <c r="F131" s="7"/>
       <c r="I131" s="3"/>
     </row>
     <row r="132" spans="1:9" ht="15" x14ac:dyDescent="0.25">
@@ -3906,6 +4241,7 @@
         <f>TblCatalogoCuentas[[#This Row],[Código]] &amp; " - " &amp; TblCatalogoCuentas[[#This Row],[Descripción]]</f>
         <v>511001 - VENTAS AL CONTADO</v>
       </c>
+      <c r="F132" s="7"/>
       <c r="H132" s="3"/>
     </row>
     <row r="133" spans="1:9" x14ac:dyDescent="0.3">
@@ -3927,6 +4263,7 @@
         <f>TblCatalogoCuentas[[#This Row],[Código]] &amp; " - " &amp; TblCatalogoCuentas[[#This Row],[Descripción]]</f>
         <v xml:space="preserve">511002 - VENTAS AL CRÉDITO </v>
       </c>
+      <c r="F133" s="7"/>
       <c r="H133" s="3"/>
     </row>
     <row r="134" spans="1:9" ht="15" x14ac:dyDescent="0.25">
@@ -3948,6 +4285,7 @@
         <f>TblCatalogoCuentas[[#This Row],[Código]] &amp; " - " &amp; TblCatalogoCuentas[[#This Row],[Descripción]]</f>
         <v xml:space="preserve">512 - REBAJAS, DEVOLUCIONES SOBRE COMPRAS </v>
       </c>
+      <c r="F134" s="7"/>
       <c r="I134" s="3"/>
     </row>
     <row r="135" spans="1:9" ht="15" x14ac:dyDescent="0.25">
@@ -3969,6 +4307,7 @@
         <f>TblCatalogoCuentas[[#This Row],[Código]] &amp; " - " &amp; TblCatalogoCuentas[[#This Row],[Descripción]]</f>
         <v>512001 - REBAJAS SOBRE COMPRAS</v>
       </c>
+      <c r="F135" s="7"/>
       <c r="H135" s="3"/>
     </row>
     <row r="136" spans="1:9" ht="15" x14ac:dyDescent="0.25">
@@ -3990,6 +4329,7 @@
         <f>TblCatalogoCuentas[[#This Row],[Código]] &amp; " - " &amp; TblCatalogoCuentas[[#This Row],[Descripción]]</f>
         <v xml:space="preserve">512002 - DEVOLUCIONES SOBRE COMPRAS  </v>
       </c>
+      <c r="F136" s="7"/>
       <c r="H136" s="3"/>
     </row>
     <row r="137" spans="1:9" ht="15" x14ac:dyDescent="0.25">
@@ -4011,6 +4351,7 @@
         <f>TblCatalogoCuentas[[#This Row],[Código]] &amp; " - " &amp; TblCatalogoCuentas[[#This Row],[Descripción]]</f>
         <v xml:space="preserve">52 - INGRESOS NO OPERACIONALES </v>
       </c>
+      <c r="F137" s="7"/>
       <c r="I137" s="2"/>
     </row>
     <row r="138" spans="1:9" ht="15" x14ac:dyDescent="0.25">
@@ -4032,6 +4373,7 @@
         <f>TblCatalogoCuentas[[#This Row],[Código]] &amp; " - " &amp; TblCatalogoCuentas[[#This Row],[Descripción]]</f>
         <v>521 - UTILIDAD POR VENTA DE PROPIEDAD, PLANTA Y EQUIPO</v>
       </c>
+      <c r="F138" s="7"/>
       <c r="I138" s="3"/>
     </row>
     <row r="139" spans="1:9" ht="15" x14ac:dyDescent="0.25">
@@ -4053,6 +4395,7 @@
         <f>TblCatalogoCuentas[[#This Row],[Código]] &amp; " - " &amp; TblCatalogoCuentas[[#This Row],[Descripción]]</f>
         <v>521001 - UTILIDAD POR VENTA BIENES INMUEBLES</v>
       </c>
+      <c r="F139" s="7"/>
       <c r="H139" s="3"/>
     </row>
     <row r="140" spans="1:9" ht="15" x14ac:dyDescent="0.25">
@@ -4074,6 +4417,7 @@
         <f>TblCatalogoCuentas[[#This Row],[Código]] &amp; " - " &amp; TblCatalogoCuentas[[#This Row],[Descripción]]</f>
         <v>521002 - UTILIDAD POR VENTA BIENES MUEBLES</v>
       </c>
+      <c r="F140" s="7"/>
       <c r="H140" s="3"/>
     </row>
     <row r="141" spans="1:9" ht="15" x14ac:dyDescent="0.25">
@@ -4095,6 +4439,7 @@
         <f>TblCatalogoCuentas[[#This Row],[Código]] &amp; " - " &amp; TblCatalogoCuentas[[#This Row],[Descripción]]</f>
         <v>522 - OTROS INGRESOS NO OPERACIONALES</v>
       </c>
+      <c r="F141" s="7"/>
       <c r="I141" s="3"/>
     </row>
     <row r="142" spans="1:9" ht="15" x14ac:dyDescent="0.25">
@@ -4116,6 +4461,7 @@
         <f>TblCatalogoCuentas[[#This Row],[Código]] &amp; " - " &amp; TblCatalogoCuentas[[#This Row],[Descripción]]</f>
         <v>522001 - INTERESES</v>
       </c>
+      <c r="F142" s="7"/>
       <c r="H142" s="3"/>
     </row>
     <row r="143" spans="1:9" ht="15" x14ac:dyDescent="0.25">
@@ -4137,6 +4483,7 @@
         <f>TblCatalogoCuentas[[#This Row],[Código]] &amp; " - " &amp; TblCatalogoCuentas[[#This Row],[Descripción]]</f>
         <v xml:space="preserve">522002 - DIVERSOS </v>
       </c>
+      <c r="F143" s="7"/>
       <c r="H143" s="3"/>
     </row>
     <row r="144" spans="1:9" ht="15" x14ac:dyDescent="0.25">
@@ -4158,6 +4505,7 @@
         <f>TblCatalogoCuentas[[#This Row],[Código]] &amp; " - " &amp; TblCatalogoCuentas[[#This Row],[Descripción]]</f>
         <v xml:space="preserve">6 - CUENTAS DE CIERRE </v>
       </c>
+      <c r="F144" s="7"/>
       <c r="I144" s="2"/>
     </row>
     <row r="145" spans="1:9" ht="15" x14ac:dyDescent="0.25">
@@ -4179,6 +4527,7 @@
         <f>TblCatalogoCuentas[[#This Row],[Código]] &amp; " - " &amp; TblCatalogoCuentas[[#This Row],[Descripción]]</f>
         <v xml:space="preserve">61 - CUENTA LIQUIDADORA </v>
       </c>
+      <c r="F145" s="7"/>
       <c r="I145" s="2"/>
     </row>
     <row r="146" spans="1:9" x14ac:dyDescent="0.3">
@@ -4200,9 +4549,15 @@
         <f>TblCatalogoCuentas[[#This Row],[Código]] &amp; " - " &amp; TblCatalogoCuentas[[#This Row],[Descripción]]</f>
         <v xml:space="preserve">611 - PÉRDIDAS Y GANANCIAS </v>
       </c>
+      <c r="F146" s="7"/>
       <c r="I146" s="3"/>
     </row>
   </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F146">
+      <formula1>TblNaturalezaCuentas_Aux</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
@@ -4353,12 +4708,21 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <sheetData>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A5" t="str">
+        <f>INDEX(TblCatalogoCuentas[], MATCH(1,TblCatalogoCuentas[Código],0), 4)</f>
+        <v xml:space="preserve">ACTIVO </v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -4367,7 +4731,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
@@ -4399,4 +4765,50 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="21.44140625" customWidth="1"/>
+    <col min="2" max="2" width="172.44140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>165</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>166</v>
+      </c>
+      <c r="B2" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>167</v>
+      </c>
+      <c r="B3" t="s">
+        <v>168</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>